<commit_message>
Savings from income and Expenses
</commit_message>
<xml_diff>
--- a/Dashboard.xlsx
+++ b/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECTS\Excel Annual budgeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F6E420-1714-489B-B70F-DB3DDF91CFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ABDAA8-C3DE-44E0-AAF0-83108F28D7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="837" activeTab="2" xr2:uid="{66796EC1-6952-4E05-AD15-9B275F7952B0}"/>
   </bookViews>
@@ -610,12 +610,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -638,6 +632,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -655,6 +652,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6630,7 +6630,7 @@
   <dimension ref="C1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="S76" sqref="S76"/>
+      <selection activeCell="N68" sqref="N68:N69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6943,51 +6943,51 @@
       </c>
       <c r="D40" s="42"/>
       <c r="E40" s="43"/>
-      <c r="F40" s="63">
+      <c r="F40" s="62">
         <f>F60</f>
         <v>7600</v>
       </c>
-      <c r="G40" s="63">
+      <c r="G40" s="62">
         <f>G60</f>
         <v>7000</v>
       </c>
-      <c r="H40" s="63">
+      <c r="H40" s="62">
         <f t="shared" ref="H40:Q40" si="0">H60</f>
         <v>7400</v>
       </c>
-      <c r="I40" s="63">
+      <c r="I40" s="62">
         <f t="shared" si="0"/>
         <v>9200</v>
       </c>
-      <c r="J40" s="63">
+      <c r="J40" s="62">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
-      <c r="K40" s="63">
+      <c r="K40" s="62">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
-      <c r="L40" s="63">
+      <c r="L40" s="62">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
-      <c r="M40" s="63">
+      <c r="M40" s="62">
         <f t="shared" si="0"/>
         <v>7100</v>
       </c>
-      <c r="N40" s="63">
+      <c r="N40" s="62">
         <f t="shared" si="0"/>
         <v>9050</v>
       </c>
-      <c r="O40" s="63">
+      <c r="O40" s="62">
         <f t="shared" si="0"/>
         <v>9250</v>
       </c>
-      <c r="P40" s="63">
+      <c r="P40" s="62">
         <f t="shared" si="0"/>
         <v>8700</v>
       </c>
-      <c r="Q40" s="63">
+      <c r="Q40" s="62">
         <f t="shared" si="0"/>
         <v>9400</v>
       </c>
@@ -6996,18 +6996,18 @@
       <c r="C41" s="44"/>
       <c r="D41" s="45"/>
       <c r="E41" s="46"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="64"/>
-      <c r="J41" s="64"/>
-      <c r="K41" s="64"/>
-      <c r="L41" s="64"/>
-      <c r="M41" s="64"/>
-      <c r="N41" s="64"/>
-      <c r="O41" s="64"/>
-      <c r="P41" s="64"/>
-      <c r="Q41" s="64"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="63"/>
+      <c r="O41" s="63"/>
+      <c r="P41" s="63"/>
+      <c r="Q41" s="63"/>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C42" s="41" t="s">
@@ -7015,35 +7015,71 @@
       </c>
       <c r="D42" s="42"/>
       <c r="E42" s="43"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
+      <c r="F42" s="58">
+        <f>F82</f>
+        <v>4560</v>
+      </c>
+      <c r="G42" s="58">
+        <f t="shared" ref="G42:Q42" si="1">G82</f>
+        <v>4465</v>
+      </c>
+      <c r="H42" s="58">
+        <f t="shared" si="1"/>
+        <v>3980</v>
+      </c>
+      <c r="I42" s="58">
+        <f t="shared" si="1"/>
+        <v>4445</v>
+      </c>
+      <c r="J42" s="58">
+        <f t="shared" si="1"/>
+        <v>4410</v>
+      </c>
+      <c r="K42" s="58">
+        <f t="shared" si="1"/>
+        <v>4015</v>
+      </c>
+      <c r="L42" s="58">
+        <f t="shared" si="1"/>
+        <v>4790</v>
+      </c>
+      <c r="M42" s="58">
+        <f t="shared" si="1"/>
+        <v>4890</v>
+      </c>
+      <c r="N42" s="58">
+        <f t="shared" si="1"/>
+        <v>4520</v>
+      </c>
+      <c r="O42" s="58">
+        <f t="shared" si="1"/>
+        <v>4460</v>
+      </c>
+      <c r="P42" s="58">
+        <f t="shared" si="1"/>
+        <v>4615</v>
+      </c>
+      <c r="Q42" s="58">
+        <f t="shared" si="1"/>
+        <v>5425</v>
+      </c>
     </row>
     <row r="43" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C43" s="44"/>
       <c r="D43" s="45"/>
       <c r="E43" s="46"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="50"/>
-      <c r="L43" s="50"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="50"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="57"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="57"/>
+      <c r="P43" s="57"/>
+      <c r="Q43" s="57"/>
     </row>
     <row r="44" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C44" s="41" t="s">
@@ -7051,35 +7087,71 @@
       </c>
       <c r="D44" s="42"/>
       <c r="E44" s="43"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="49"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49"/>
-      <c r="O44" s="49"/>
-      <c r="P44" s="49"/>
-      <c r="Q44" s="49"/>
+      <c r="F44" s="60">
+        <f>F40-F42</f>
+        <v>3040</v>
+      </c>
+      <c r="G44" s="60">
+        <f t="shared" ref="G44:Q44" si="2">G40-G42</f>
+        <v>2535</v>
+      </c>
+      <c r="H44" s="60">
+        <f t="shared" si="2"/>
+        <v>3420</v>
+      </c>
+      <c r="I44" s="60">
+        <f t="shared" si="2"/>
+        <v>4755</v>
+      </c>
+      <c r="J44" s="60">
+        <f t="shared" si="2"/>
+        <v>2590</v>
+      </c>
+      <c r="K44" s="60">
+        <f t="shared" si="2"/>
+        <v>3485</v>
+      </c>
+      <c r="L44" s="60">
+        <f t="shared" si="2"/>
+        <v>2710</v>
+      </c>
+      <c r="M44" s="60">
+        <f t="shared" si="2"/>
+        <v>2210</v>
+      </c>
+      <c r="N44" s="60">
+        <f t="shared" si="2"/>
+        <v>4530</v>
+      </c>
+      <c r="O44" s="60">
+        <f t="shared" si="2"/>
+        <v>4790</v>
+      </c>
+      <c r="P44" s="60">
+        <f t="shared" si="2"/>
+        <v>4085</v>
+      </c>
+      <c r="Q44" s="60">
+        <f t="shared" si="2"/>
+        <v>3975</v>
+      </c>
     </row>
     <row r="45" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C45" s="44"/>
       <c r="D45" s="45"/>
       <c r="E45" s="46"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="50"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="50"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="50"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="64"/>
+      <c r="L45" s="64"/>
+      <c r="M45" s="64"/>
+      <c r="N45" s="64"/>
+      <c r="O45" s="64"/>
+      <c r="P45" s="64"/>
+      <c r="Q45" s="64"/>
     </row>
     <row r="47" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="48" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7094,8 +7166,8 @@
       <c r="C50" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="51"/>
-      <c r="E50" s="52"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="50"/>
       <c r="F50" s="47" t="s">
         <v>31</v>
       </c>
@@ -7134,9 +7206,9 @@
       </c>
     </row>
     <row r="51" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C51" s="53"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="55"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="53"/>
       <c r="F51" s="48"/>
       <c r="G51" s="48"/>
       <c r="H51" s="48"/>
@@ -7156,51 +7228,51 @@
       </c>
       <c r="D52" s="42"/>
       <c r="E52" s="43"/>
-      <c r="F52" s="59">
+      <c r="F52" s="58">
         <f>VLOOKUP(F50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="G52" s="59">
+      <c r="G52" s="58">
         <f>VLOOKUP(G50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="H52" s="59">
+      <c r="H52" s="58">
         <f>VLOOKUP(H50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="I52" s="59">
+      <c r="I52" s="58">
         <f>VLOOKUP(I50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>7500</v>
       </c>
-      <c r="J52" s="59">
+      <c r="J52" s="58">
         <f>VLOOKUP(J50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="K52" s="59">
+      <c r="K52" s="58">
         <f>VLOOKUP(K50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="L52" s="59">
+      <c r="L52" s="58">
         <f>VLOOKUP(L50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="M52" s="59">
+      <c r="M52" s="58">
         <f>VLOOKUP(M50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="N52" s="59">
+      <c r="N52" s="58">
         <f>VLOOKUP(N50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="O52" s="59">
+      <c r="O52" s="58">
         <f>VLOOKUP(O50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="P52" s="59">
+      <c r="P52" s="58">
         <f>VLOOKUP(P50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="Q52" s="59">
+      <c r="Q52" s="58">
         <f>VLOOKUP(Q50,Income!$D$7:$H$19,2,FALSE)</f>
         <v>6000</v>
       </c>
@@ -7209,18 +7281,18 @@
       <c r="C53" s="44"/>
       <c r="D53" s="45"/>
       <c r="E53" s="46"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
-      <c r="H53" s="60"/>
-      <c r="I53" s="60"/>
-      <c r="J53" s="60"/>
-      <c r="K53" s="60"/>
-      <c r="L53" s="60"/>
-      <c r="M53" s="60"/>
-      <c r="N53" s="60"/>
-      <c r="O53" s="60"/>
-      <c r="P53" s="60"/>
-      <c r="Q53" s="60"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="59"/>
+      <c r="K53" s="59"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="59"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="59"/>
     </row>
     <row r="54" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C54" s="41" t="s">
@@ -7228,51 +7300,51 @@
       </c>
       <c r="D54" s="42"/>
       <c r="E54" s="43"/>
-      <c r="F54" s="59">
+      <c r="F54" s="58">
         <f>VLOOKUP(F50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>200</v>
       </c>
-      <c r="G54" s="59">
+      <c r="G54" s="58">
         <f>VLOOKUP(G50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>100</v>
       </c>
-      <c r="H54" s="59">
+      <c r="H54" s="58">
         <f>VLOOKUP(H50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>500</v>
       </c>
-      <c r="I54" s="59">
+      <c r="I54" s="58">
         <f>VLOOKUP(I50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="J54" s="59">
+      <c r="J54" s="58">
         <f>VLOOKUP(J50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="K54" s="59">
+      <c r="K54" s="58">
         <f>VLOOKUP(K50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="L54" s="59">
+      <c r="L54" s="58">
         <f>VLOOKUP(L50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>400</v>
       </c>
-      <c r="M54" s="59">
+      <c r="M54" s="58">
         <f>VLOOKUP(M50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>200</v>
       </c>
-      <c r="N54" s="59">
+      <c r="N54" s="58">
         <f>VLOOKUP(N50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>850</v>
       </c>
-      <c r="O54" s="59">
+      <c r="O54" s="58">
         <f>VLOOKUP(O50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>950</v>
       </c>
-      <c r="P54" s="59">
+      <c r="P54" s="58">
         <f>VLOOKUP(P50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>600</v>
       </c>
-      <c r="Q54" s="59">
+      <c r="Q54" s="58">
         <f>VLOOKUP(Q50,Income!$D$7:$H$19,3,FALSE)</f>
         <v>700</v>
       </c>
@@ -7281,18 +7353,18 @@
       <c r="C55" s="44"/>
       <c r="D55" s="45"/>
       <c r="E55" s="46"/>
-      <c r="F55" s="60"/>
-      <c r="G55" s="60"/>
-      <c r="H55" s="60"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-      <c r="K55" s="60"/>
-      <c r="L55" s="60"/>
-      <c r="M55" s="60"/>
-      <c r="N55" s="60"/>
-      <c r="O55" s="60"/>
-      <c r="P55" s="60"/>
-      <c r="Q55" s="60"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="59"/>
+      <c r="K55" s="59"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="59"/>
+      <c r="Q55" s="59"/>
     </row>
     <row r="56" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C56" s="41" t="s">
@@ -7300,51 +7372,51 @@
       </c>
       <c r="D56" s="42"/>
       <c r="E56" s="43"/>
-      <c r="F56" s="59">
+      <c r="F56" s="58">
         <f>VLOOKUP(F50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>1200</v>
       </c>
-      <c r="G56" s="59">
+      <c r="G56" s="58">
         <f>VLOOKUP(G50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>800</v>
       </c>
-      <c r="H56" s="59">
+      <c r="H56" s="58">
         <f>VLOOKUP(H50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>900</v>
       </c>
-      <c r="I56" s="59">
+      <c r="I56" s="58">
         <f>VLOOKUP(I50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>900</v>
       </c>
-      <c r="J56" s="59">
+      <c r="J56" s="58">
         <f>VLOOKUP(J50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>900</v>
       </c>
-      <c r="K56" s="59">
+      <c r="K56" s="58">
         <f>VLOOKUP(K50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="L56" s="59">
+      <c r="L56" s="58">
         <f>VLOOKUP(L50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="M56" s="59">
+      <c r="M56" s="58">
         <f>VLOOKUP(M50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="N56" s="59">
+      <c r="N56" s="58">
         <f>VLOOKUP(N50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>1500</v>
       </c>
-      <c r="O56" s="59">
+      <c r="O56" s="58">
         <f>VLOOKUP(O50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>1600</v>
       </c>
-      <c r="P56" s="59">
+      <c r="P56" s="58">
         <f>VLOOKUP(P50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>1500</v>
       </c>
-      <c r="Q56" s="59">
+      <c r="Q56" s="58">
         <f>VLOOKUP(Q50,Income!$D$7:$H$19,4,FALSE)</f>
         <v>700</v>
       </c>
@@ -7353,18 +7425,18 @@
       <c r="C57" s="44"/>
       <c r="D57" s="45"/>
       <c r="E57" s="46"/>
-      <c r="F57" s="60"/>
-      <c r="G57" s="60"/>
-      <c r="H57" s="60"/>
-      <c r="I57" s="60"/>
-      <c r="J57" s="60"/>
-      <c r="K57" s="60"/>
-      <c r="L57" s="60"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="60"/>
-      <c r="O57" s="60"/>
-      <c r="P57" s="60"/>
-      <c r="Q57" s="60"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="59"/>
+      <c r="K57" s="59"/>
+      <c r="L57" s="59"/>
+      <c r="M57" s="59"/>
+      <c r="N57" s="59"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="59"/>
+      <c r="Q57" s="59"/>
     </row>
     <row r="58" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C58" s="41" t="s">
@@ -7372,51 +7444,51 @@
       </c>
       <c r="D58" s="42"/>
       <c r="E58" s="43"/>
-      <c r="F58" s="59">
+      <c r="F58" s="58">
         <f>VLOOKUP(F50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>1200</v>
       </c>
-      <c r="G58" s="59">
+      <c r="G58" s="58">
         <f>VLOOKUP(G50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>1100</v>
       </c>
-      <c r="H58" s="59">
+      <c r="H58" s="58">
         <f>VLOOKUP(H50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>1000</v>
       </c>
-      <c r="I58" s="59">
+      <c r="I58" s="58">
         <f>VLOOKUP(I50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>800</v>
       </c>
-      <c r="J58" s="59">
+      <c r="J58" s="58">
         <f>VLOOKUP(J50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>800</v>
       </c>
-      <c r="K58" s="59">
+      <c r="K58" s="58">
         <f>VLOOKUP(K50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>2200</v>
       </c>
-      <c r="L58" s="59">
+      <c r="L58" s="58">
         <f>VLOOKUP(L50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>2100</v>
       </c>
-      <c r="M58" s="59">
+      <c r="M58" s="58">
         <f>VLOOKUP(M50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>1900</v>
       </c>
-      <c r="N58" s="59">
+      <c r="N58" s="58">
         <f>VLOOKUP(N50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>1700</v>
       </c>
-      <c r="O58" s="59">
+      <c r="O58" s="58">
         <f>VLOOKUP(O50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>1700</v>
       </c>
-      <c r="P58" s="59">
+      <c r="P58" s="58">
         <f>VLOOKUP(P50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>1600</v>
       </c>
-      <c r="Q58" s="59">
+      <c r="Q58" s="58">
         <f>VLOOKUP(Q50,Income!$D$7:$H$19,5,FALSE)</f>
         <v>2000</v>
       </c>
@@ -7425,106 +7497,106 @@
       <c r="C59" s="44"/>
       <c r="D59" s="45"/>
       <c r="E59" s="46"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="60"/>
-      <c r="J59" s="60"/>
-      <c r="K59" s="60"/>
-      <c r="L59" s="60"/>
-      <c r="M59" s="60"/>
-      <c r="N59" s="60"/>
-      <c r="O59" s="60"/>
-      <c r="P59" s="60"/>
-      <c r="Q59" s="60"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="59"/>
+      <c r="K59" s="59"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="59"/>
     </row>
     <row r="60" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C60" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D60" s="51"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="61">
+      <c r="D60" s="49"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="60">
         <f>SUM(F52:F58)</f>
         <v>7600</v>
       </c>
-      <c r="G60" s="61">
-        <f t="shared" ref="G60:Q60" si="1">SUM(G52:G58)</f>
+      <c r="G60" s="60">
+        <f t="shared" ref="G60:Q60" si="3">SUM(G52:G58)</f>
         <v>7000</v>
       </c>
-      <c r="H60" s="61">
-        <f t="shared" si="1"/>
+      <c r="H60" s="60">
+        <f t="shared" si="3"/>
         <v>7400</v>
       </c>
-      <c r="I60" s="61">
-        <f t="shared" si="1"/>
+      <c r="I60" s="60">
+        <f t="shared" si="3"/>
         <v>9200</v>
       </c>
-      <c r="J60" s="61">
-        <f t="shared" si="1"/>
+      <c r="J60" s="60">
+        <f t="shared" si="3"/>
         <v>7000</v>
       </c>
-      <c r="K60" s="61">
-        <f t="shared" si="1"/>
+      <c r="K60" s="60">
+        <f t="shared" si="3"/>
         <v>7500</v>
       </c>
-      <c r="L60" s="61">
-        <f t="shared" si="1"/>
+      <c r="L60" s="60">
+        <f t="shared" si="3"/>
         <v>7500</v>
       </c>
-      <c r="M60" s="61">
-        <f t="shared" si="1"/>
+      <c r="M60" s="60">
+        <f t="shared" si="3"/>
         <v>7100</v>
       </c>
-      <c r="N60" s="61">
-        <f t="shared" si="1"/>
+      <c r="N60" s="60">
+        <f t="shared" si="3"/>
         <v>9050</v>
       </c>
-      <c r="O60" s="61">
-        <f t="shared" si="1"/>
+      <c r="O60" s="60">
+        <f t="shared" si="3"/>
         <v>9250</v>
       </c>
-      <c r="P60" s="61">
-        <f t="shared" si="1"/>
+      <c r="P60" s="60">
+        <f t="shared" si="3"/>
         <v>8700</v>
       </c>
-      <c r="Q60" s="61">
-        <f t="shared" si="1"/>
+      <c r="Q60" s="60">
+        <f t="shared" si="3"/>
         <v>9400</v>
       </c>
     </row>
     <row r="61" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C61" s="53"/>
-      <c r="D61" s="54"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="62"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="62"/>
-      <c r="J61" s="62"/>
-      <c r="K61" s="62"/>
-      <c r="L61" s="62"/>
-      <c r="M61" s="62"/>
-      <c r="N61" s="62"/>
-      <c r="O61" s="62"/>
-      <c r="P61" s="62"/>
-      <c r="Q61" s="62"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="61"/>
+      <c r="G61" s="61"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="61"/>
+      <c r="J61" s="61"/>
+      <c r="K61" s="61"/>
+      <c r="L61" s="61"/>
+      <c r="M61" s="61"/>
+      <c r="N61" s="61"/>
+      <c r="O61" s="61"/>
+      <c r="P61" s="61"/>
+      <c r="Q61" s="61"/>
     </row>
     <row r="63" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="64" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C64" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="56"/>
-      <c r="E64" s="57"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="55"/>
     </row>
     <row r="65" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="66" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C66" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="51"/>
-      <c r="E66" s="52"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="50"/>
       <c r="F66" s="47" t="s">
         <v>31</v>
       </c>
@@ -7563,9 +7635,9 @@
       </c>
     </row>
     <row r="67" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C67" s="53"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="55"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="53"/>
       <c r="F67" s="48"/>
       <c r="G67" s="48"/>
       <c r="H67" s="48"/>
@@ -7585,51 +7657,51 @@
       </c>
       <c r="D68" s="42"/>
       <c r="E68" s="43"/>
-      <c r="F68" s="59">
+      <c r="F68" s="58">
         <f>_xlfn.XLOOKUP(F66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2100</v>
       </c>
-      <c r="G68" s="59">
+      <c r="G68" s="58">
         <f>_xlfn.XLOOKUP(G66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2100</v>
       </c>
-      <c r="H68" s="59">
+      <c r="H68" s="58">
         <f>_xlfn.XLOOKUP(H66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2100</v>
       </c>
-      <c r="I68" s="59">
+      <c r="I68" s="58">
         <f>_xlfn.XLOOKUP(I66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2100</v>
       </c>
-      <c r="J68" s="59">
+      <c r="J68" s="58">
         <f>_xlfn.XLOOKUP(J66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2100</v>
       </c>
-      <c r="K68" s="59">
+      <c r="K68" s="58">
         <f>_xlfn.XLOOKUP(K66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2100</v>
       </c>
-      <c r="L68" s="59">
+      <c r="L68" s="58">
         <f>_xlfn.XLOOKUP(L66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2350</v>
       </c>
-      <c r="M68" s="59">
+      <c r="M68" s="58">
         <f>_xlfn.XLOOKUP(M66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2350</v>
       </c>
-      <c r="N68" s="59">
+      <c r="N68" s="58">
         <f>_xlfn.XLOOKUP(N66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2350</v>
       </c>
-      <c r="O68" s="59">
+      <c r="O68" s="58">
         <f>_xlfn.XLOOKUP(O66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2350</v>
       </c>
-      <c r="P68" s="59">
+      <c r="P68" s="58">
         <f>_xlfn.XLOOKUP(P66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2350</v>
       </c>
-      <c r="Q68" s="59">
+      <c r="Q68" s="58">
         <f>_xlfn.XLOOKUP(Q66,Expenses!$D$9:$D$20,Expenses!$E$9:$E$20)</f>
         <v>2350</v>
       </c>
@@ -7638,18 +7710,18 @@
       <c r="C69" s="44"/>
       <c r="D69" s="45"/>
       <c r="E69" s="46"/>
-      <c r="F69" s="60"/>
-      <c r="G69" s="60"/>
-      <c r="H69" s="60"/>
-      <c r="I69" s="60"/>
-      <c r="J69" s="60"/>
-      <c r="K69" s="60"/>
-      <c r="L69" s="60"/>
-      <c r="M69" s="60"/>
-      <c r="N69" s="60"/>
-      <c r="O69" s="60"/>
-      <c r="P69" s="60"/>
-      <c r="Q69" s="60"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="59"/>
+      <c r="J69" s="59"/>
+      <c r="K69" s="59"/>
+      <c r="L69" s="59"/>
+      <c r="M69" s="59"/>
+      <c r="N69" s="59"/>
+      <c r="O69" s="59"/>
+      <c r="P69" s="59"/>
+      <c r="Q69" s="59"/>
     </row>
     <row r="70" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C70" s="41" t="s">
@@ -7657,51 +7729,51 @@
       </c>
       <c r="D70" s="42"/>
       <c r="E70" s="43"/>
-      <c r="F70" s="59">
+      <c r="F70" s="58">
         <f>_xlfn.XLOOKUP(F66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="G70" s="59">
+      <c r="G70" s="58">
         <f>_xlfn.XLOOKUP(G66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="H70" s="59">
+      <c r="H70" s="58">
         <f>_xlfn.XLOOKUP(H66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="I70" s="59">
+      <c r="I70" s="58">
         <f>_xlfn.XLOOKUP(I66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="J70" s="59">
+      <c r="J70" s="58">
         <f>_xlfn.XLOOKUP(J66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="K70" s="59">
+      <c r="K70" s="58">
         <f>_xlfn.XLOOKUP(K66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="L70" s="59">
+      <c r="L70" s="58">
         <f>_xlfn.XLOOKUP(L66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="M70" s="59">
+      <c r="M70" s="58">
         <f>_xlfn.XLOOKUP(M66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="N70" s="59">
+      <c r="N70" s="58">
         <f>_xlfn.XLOOKUP(N66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="O70" s="59">
+      <c r="O70" s="58">
         <f>_xlfn.XLOOKUP(O66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
-      <c r="P70" s="59">
+      <c r="P70" s="58">
         <f>_xlfn.XLOOKUP(P66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>400</v>
       </c>
-      <c r="Q70" s="59">
+      <c r="Q70" s="58">
         <f>_xlfn.XLOOKUP(Q66,Expenses!$D$9:$D$20,Expenses!$F$9:$F$20)</f>
         <v>300</v>
       </c>
@@ -7710,18 +7782,18 @@
       <c r="C71" s="44"/>
       <c r="D71" s="45"/>
       <c r="E71" s="46"/>
-      <c r="F71" s="60"/>
-      <c r="G71" s="60"/>
-      <c r="H71" s="60"/>
-      <c r="I71" s="60"/>
-      <c r="J71" s="60"/>
-      <c r="K71" s="60"/>
-      <c r="L71" s="60"/>
-      <c r="M71" s="60"/>
-      <c r="N71" s="60"/>
-      <c r="O71" s="60"/>
-      <c r="P71" s="60"/>
-      <c r="Q71" s="60"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="59"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="59"/>
+      <c r="L71" s="59"/>
+      <c r="M71" s="59"/>
+      <c r="N71" s="59"/>
+      <c r="O71" s="59"/>
+      <c r="P71" s="59"/>
+      <c r="Q71" s="59"/>
     </row>
     <row r="72" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C72" s="41" t="s">
@@ -7729,51 +7801,51 @@
       </c>
       <c r="D72" s="42"/>
       <c r="E72" s="43"/>
-      <c r="F72" s="59">
+      <c r="F72" s="58">
         <f>_xlfn.XLOOKUP(F66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>225</v>
       </c>
-      <c r="G72" s="59">
+      <c r="G72" s="58">
         <f>_xlfn.XLOOKUP(G66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>225</v>
       </c>
-      <c r="H72" s="59">
+      <c r="H72" s="58">
         <f>_xlfn.XLOOKUP(H66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>150</v>
       </c>
-      <c r="I72" s="59">
+      <c r="I72" s="58">
         <f>_xlfn.XLOOKUP(I66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>150</v>
       </c>
-      <c r="J72" s="59">
+      <c r="J72" s="58">
         <f>_xlfn.XLOOKUP(J66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>300</v>
       </c>
-      <c r="K72" s="59">
+      <c r="K72" s="58">
         <f>_xlfn.XLOOKUP(K66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>225</v>
       </c>
-      <c r="L72" s="59">
+      <c r="L72" s="58">
         <f>_xlfn.XLOOKUP(L66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>225</v>
       </c>
-      <c r="M72" s="59">
+      <c r="M72" s="58">
         <f>_xlfn.XLOOKUP(M66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>150</v>
       </c>
-      <c r="N72" s="59">
+      <c r="N72" s="58">
         <f>_xlfn.XLOOKUP(N66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>300</v>
       </c>
-      <c r="O72" s="59">
+      <c r="O72" s="58">
         <f>_xlfn.XLOOKUP(O66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>225</v>
       </c>
-      <c r="P72" s="59">
+      <c r="P72" s="58">
         <f>_xlfn.XLOOKUP(P66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>225</v>
       </c>
-      <c r="Q72" s="59">
+      <c r="Q72" s="58">
         <f>_xlfn.XLOOKUP(Q66,Expenses!$D$9:$D$20,Expenses!$G$9:$G$20)</f>
         <v>300</v>
       </c>
@@ -7782,18 +7854,18 @@
       <c r="C73" s="44"/>
       <c r="D73" s="45"/>
       <c r="E73" s="46"/>
-      <c r="F73" s="60"/>
-      <c r="G73" s="60"/>
-      <c r="H73" s="60"/>
-      <c r="I73" s="60"/>
-      <c r="J73" s="60"/>
-      <c r="K73" s="60"/>
-      <c r="L73" s="60"/>
-      <c r="M73" s="60"/>
-      <c r="N73" s="60"/>
-      <c r="O73" s="60"/>
-      <c r="P73" s="60"/>
-      <c r="Q73" s="60"/>
+      <c r="F73" s="59"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="59"/>
+      <c r="J73" s="59"/>
+      <c r="K73" s="59"/>
+      <c r="L73" s="59"/>
+      <c r="M73" s="59"/>
+      <c r="N73" s="59"/>
+      <c r="O73" s="59"/>
+      <c r="P73" s="59"/>
+      <c r="Q73" s="59"/>
     </row>
     <row r="74" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C74" s="41" t="s">
@@ -7801,51 +7873,51 @@
       </c>
       <c r="D74" s="42"/>
       <c r="E74" s="43"/>
-      <c r="F74" s="59">
+      <c r="F74" s="58">
         <f>_xlfn.XLOOKUP(F66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>400</v>
       </c>
-      <c r="G74" s="59">
+      <c r="G74" s="58">
         <f>_xlfn.XLOOKUP(G66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>300</v>
       </c>
-      <c r="H74" s="59">
+      <c r="H74" s="58">
         <f>_xlfn.XLOOKUP(H66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>100</v>
       </c>
-      <c r="I74" s="59">
+      <c r="I74" s="58">
         <f>_xlfn.XLOOKUP(I66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>500</v>
       </c>
-      <c r="J74" s="59">
+      <c r="J74" s="58">
         <f>_xlfn.XLOOKUP(J66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>300</v>
       </c>
-      <c r="K74" s="59">
+      <c r="K74" s="58">
         <f>_xlfn.XLOOKUP(K66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>300</v>
       </c>
-      <c r="L74" s="59">
+      <c r="L74" s="58">
         <f>_xlfn.XLOOKUP(L66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>150</v>
       </c>
-      <c r="M74" s="59">
+      <c r="M74" s="58">
         <f>_xlfn.XLOOKUP(M66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>200</v>
       </c>
-      <c r="N74" s="59">
+      <c r="N74" s="58">
         <f>_xlfn.XLOOKUP(N66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>200</v>
       </c>
-      <c r="O74" s="59">
+      <c r="O74" s="58">
         <f>_xlfn.XLOOKUP(O66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>500</v>
       </c>
-      <c r="P74" s="59">
+      <c r="P74" s="58">
         <f>_xlfn.XLOOKUP(P66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>200</v>
       </c>
-      <c r="Q74" s="59">
+      <c r="Q74" s="58">
         <f>_xlfn.XLOOKUP(Q66,Expenses!$D$9:$D$20,Expenses!$H$9:$H$20)</f>
         <v>100</v>
       </c>
@@ -7854,18 +7926,18 @@
       <c r="C75" s="44"/>
       <c r="D75" s="45"/>
       <c r="E75" s="46"/>
-      <c r="F75" s="60"/>
-      <c r="G75" s="60"/>
-      <c r="H75" s="60"/>
-      <c r="I75" s="60"/>
-      <c r="J75" s="60"/>
-      <c r="K75" s="60"/>
-      <c r="L75" s="60"/>
-      <c r="M75" s="60"/>
-      <c r="N75" s="60"/>
-      <c r="O75" s="60"/>
-      <c r="P75" s="60"/>
-      <c r="Q75" s="60"/>
+      <c r="F75" s="59"/>
+      <c r="G75" s="59"/>
+      <c r="H75" s="59"/>
+      <c r="I75" s="59"/>
+      <c r="J75" s="59"/>
+      <c r="K75" s="59"/>
+      <c r="L75" s="59"/>
+      <c r="M75" s="59"/>
+      <c r="N75" s="59"/>
+      <c r="O75" s="59"/>
+      <c r="P75" s="59"/>
+      <c r="Q75" s="59"/>
     </row>
     <row r="76" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C76" s="41" t="s">
@@ -7873,51 +7945,51 @@
       </c>
       <c r="D76" s="42"/>
       <c r="E76" s="43"/>
-      <c r="F76" s="59">
+      <c r="F76" s="58">
         <f>_xlfn.XLOOKUP(F66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>650</v>
       </c>
-      <c r="G76" s="59">
+      <c r="G76" s="58">
         <f>_xlfn.XLOOKUP(G66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>560</v>
       </c>
-      <c r="H76" s="59">
+      <c r="H76" s="58">
         <f>_xlfn.XLOOKUP(H66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>575</v>
       </c>
-      <c r="I76" s="59">
+      <c r="I76" s="58">
         <f>_xlfn.XLOOKUP(I66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>620</v>
       </c>
-      <c r="J76" s="59">
+      <c r="J76" s="58">
         <f>_xlfn.XLOOKUP(J66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>650</v>
       </c>
-      <c r="K76" s="59">
+      <c r="K76" s="58">
         <f>_xlfn.XLOOKUP(K66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>500</v>
       </c>
-      <c r="L76" s="59">
+      <c r="L76" s="58">
         <f>_xlfn.XLOOKUP(L66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>650</v>
       </c>
-      <c r="M76" s="59">
+      <c r="M76" s="58">
         <f>_xlfn.XLOOKUP(M66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>650</v>
       </c>
-      <c r="N76" s="59">
+      <c r="N76" s="58">
         <f>_xlfn.XLOOKUP(N66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>600</v>
       </c>
-      <c r="O76" s="59">
+      <c r="O76" s="58">
         <f>_xlfn.XLOOKUP(O66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>475</v>
       </c>
-      <c r="P76" s="59">
+      <c r="P76" s="58">
         <f>_xlfn.XLOOKUP(P66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>600</v>
       </c>
-      <c r="Q76" s="59">
+      <c r="Q76" s="58">
         <f>_xlfn.XLOOKUP(Q66,Expenses!$D$9:$D$20,Expenses!$I$9:$I$20)</f>
         <v>550</v>
       </c>
@@ -7926,18 +7998,18 @@
       <c r="C77" s="44"/>
       <c r="D77" s="45"/>
       <c r="E77" s="46"/>
-      <c r="F77" s="60"/>
-      <c r="G77" s="60"/>
-      <c r="H77" s="60"/>
-      <c r="I77" s="60"/>
-      <c r="J77" s="60"/>
-      <c r="K77" s="60"/>
-      <c r="L77" s="60"/>
-      <c r="M77" s="60"/>
-      <c r="N77" s="60"/>
-      <c r="O77" s="60"/>
-      <c r="P77" s="60"/>
-      <c r="Q77" s="60"/>
+      <c r="F77" s="59"/>
+      <c r="G77" s="59"/>
+      <c r="H77" s="59"/>
+      <c r="I77" s="59"/>
+      <c r="J77" s="59"/>
+      <c r="K77" s="59"/>
+      <c r="L77" s="59"/>
+      <c r="M77" s="59"/>
+      <c r="N77" s="59"/>
+      <c r="O77" s="59"/>
+      <c r="P77" s="59"/>
+      <c r="Q77" s="59"/>
     </row>
     <row r="78" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C78" s="41" t="s">
@@ -7945,51 +8017,51 @@
       </c>
       <c r="D78" s="42"/>
       <c r="E78" s="43"/>
-      <c r="F78" s="59">
+      <c r="F78" s="58">
         <f>_xlfn.XLOOKUP(F66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>410</v>
       </c>
-      <c r="G78" s="59">
+      <c r="G78" s="58">
         <f>_xlfn.XLOOKUP(G66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>430</v>
       </c>
-      <c r="H78" s="59">
+      <c r="H78" s="58">
         <f>_xlfn.XLOOKUP(H66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>380</v>
       </c>
-      <c r="I78" s="59">
+      <c r="I78" s="58">
         <f>_xlfn.XLOOKUP(I66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>350</v>
       </c>
-      <c r="J78" s="59">
+      <c r="J78" s="58">
         <f>_xlfn.XLOOKUP(J66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>330</v>
       </c>
-      <c r="K78" s="59">
+      <c r="K78" s="58">
         <f>_xlfn.XLOOKUP(K66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>290</v>
       </c>
-      <c r="L78" s="59">
+      <c r="L78" s="58">
         <f>_xlfn.XLOOKUP(L66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>340</v>
       </c>
-      <c r="M78" s="59">
+      <c r="M78" s="58">
         <f>_xlfn.XLOOKUP(M66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>340</v>
       </c>
-      <c r="N78" s="59">
+      <c r="N78" s="58">
         <f>_xlfn.XLOOKUP(N66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>320</v>
       </c>
-      <c r="O78" s="59">
+      <c r="O78" s="58">
         <f>_xlfn.XLOOKUP(O66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>310</v>
       </c>
-      <c r="P78" s="59">
+      <c r="P78" s="58">
         <f>_xlfn.XLOOKUP(P66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>290</v>
       </c>
-      <c r="Q78" s="59">
+      <c r="Q78" s="58">
         <f>_xlfn.XLOOKUP(Q66,Expenses!$D$9:$D$20,Expenses!$J$9:$J$20)</f>
         <v>425</v>
       </c>
@@ -7998,18 +8070,18 @@
       <c r="C79" s="44"/>
       <c r="D79" s="45"/>
       <c r="E79" s="46"/>
-      <c r="F79" s="60"/>
-      <c r="G79" s="60"/>
-      <c r="H79" s="60"/>
-      <c r="I79" s="60"/>
-      <c r="J79" s="60"/>
-      <c r="K79" s="60"/>
-      <c r="L79" s="60"/>
-      <c r="M79" s="60"/>
-      <c r="N79" s="60"/>
-      <c r="O79" s="60"/>
-      <c r="P79" s="60"/>
-      <c r="Q79" s="60"/>
+      <c r="F79" s="59"/>
+      <c r="G79" s="59"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="59"/>
+      <c r="J79" s="59"/>
+      <c r="K79" s="59"/>
+      <c r="L79" s="59"/>
+      <c r="M79" s="59"/>
+      <c r="N79" s="59"/>
+      <c r="O79" s="59"/>
+      <c r="P79" s="59"/>
+      <c r="Q79" s="59"/>
     </row>
     <row r="80" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C80" s="41" t="s">
@@ -8017,51 +8089,51 @@
       </c>
       <c r="D80" s="42"/>
       <c r="E80" s="43"/>
-      <c r="F80" s="59">
+      <c r="F80" s="58">
         <f>_xlfn.XLOOKUP(F66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>475</v>
       </c>
-      <c r="G80" s="59">
+      <c r="G80" s="58">
         <f>_xlfn.XLOOKUP(G66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>550</v>
       </c>
-      <c r="H80" s="59">
+      <c r="H80" s="58">
         <f>_xlfn.XLOOKUP(H66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>375</v>
       </c>
-      <c r="I80" s="59">
+      <c r="I80" s="58">
         <f>_xlfn.XLOOKUP(I66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>425</v>
       </c>
-      <c r="J80" s="59">
+      <c r="J80" s="58">
         <f>_xlfn.XLOOKUP(J66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>430</v>
       </c>
-      <c r="K80" s="59">
+      <c r="K80" s="58">
         <f>_xlfn.XLOOKUP(K66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>300</v>
       </c>
-      <c r="L80" s="59">
+      <c r="L80" s="58">
         <f>_xlfn.XLOOKUP(L66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>775</v>
       </c>
-      <c r="M80" s="59">
+      <c r="M80" s="58">
         <f>_xlfn.XLOOKUP(M66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>900</v>
       </c>
-      <c r="N80" s="59">
+      <c r="N80" s="58">
         <f>_xlfn.XLOOKUP(N66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>450</v>
       </c>
-      <c r="O80" s="59">
+      <c r="O80" s="58">
         <f>_xlfn.XLOOKUP(O66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>300</v>
       </c>
-      <c r="P80" s="59">
+      <c r="P80" s="58">
         <f>_xlfn.XLOOKUP(P66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>550</v>
       </c>
-      <c r="Q80" s="59">
+      <c r="Q80" s="58">
         <f>_xlfn.XLOOKUP(Q66,Expenses!$D$9:$D$20,Expenses!$K$9:$K$20)</f>
         <v>1400</v>
       </c>
@@ -8070,90 +8142,90 @@
       <c r="C81" s="44"/>
       <c r="D81" s="45"/>
       <c r="E81" s="46"/>
-      <c r="F81" s="60"/>
-      <c r="G81" s="60"/>
-      <c r="H81" s="60"/>
-      <c r="I81" s="60"/>
-      <c r="J81" s="60"/>
-      <c r="K81" s="60"/>
-      <c r="L81" s="60"/>
-      <c r="M81" s="60"/>
-      <c r="N81" s="60"/>
-      <c r="O81" s="60"/>
-      <c r="P81" s="60"/>
-      <c r="Q81" s="60"/>
+      <c r="F81" s="59"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="59"/>
+      <c r="I81" s="59"/>
+      <c r="J81" s="59"/>
+      <c r="K81" s="59"/>
+      <c r="L81" s="59"/>
+      <c r="M81" s="59"/>
+      <c r="N81" s="59"/>
+      <c r="O81" s="59"/>
+      <c r="P81" s="59"/>
+      <c r="Q81" s="59"/>
     </row>
     <row r="82" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C82" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="51"/>
-      <c r="E82" s="52"/>
-      <c r="F82" s="61">
+      <c r="D82" s="49"/>
+      <c r="E82" s="50"/>
+      <c r="F82" s="60">
         <f>SUM(F68:F81)</f>
         <v>4560</v>
       </c>
-      <c r="G82" s="61">
-        <f t="shared" ref="G82:Q82" si="2">SUM(G68:G81)</f>
+      <c r="G82" s="60">
+        <f t="shared" ref="G82:Q82" si="4">SUM(G68:G81)</f>
         <v>4465</v>
       </c>
-      <c r="H82" s="61">
-        <f t="shared" si="2"/>
+      <c r="H82" s="60">
+        <f t="shared" si="4"/>
         <v>3980</v>
       </c>
-      <c r="I82" s="61">
-        <f t="shared" si="2"/>
+      <c r="I82" s="60">
+        <f t="shared" si="4"/>
         <v>4445</v>
       </c>
-      <c r="J82" s="61">
-        <f t="shared" si="2"/>
+      <c r="J82" s="60">
+        <f t="shared" si="4"/>
         <v>4410</v>
       </c>
-      <c r="K82" s="61">
-        <f t="shared" si="2"/>
+      <c r="K82" s="60">
+        <f t="shared" si="4"/>
         <v>4015</v>
       </c>
-      <c r="L82" s="61">
-        <f t="shared" si="2"/>
+      <c r="L82" s="60">
+        <f t="shared" si="4"/>
         <v>4790</v>
       </c>
-      <c r="M82" s="61">
-        <f t="shared" si="2"/>
+      <c r="M82" s="60">
+        <f t="shared" si="4"/>
         <v>4890</v>
       </c>
-      <c r="N82" s="61">
-        <f t="shared" si="2"/>
+      <c r="N82" s="60">
+        <f t="shared" si="4"/>
         <v>4520</v>
       </c>
-      <c r="O82" s="61">
-        <f t="shared" si="2"/>
+      <c r="O82" s="60">
+        <f t="shared" si="4"/>
         <v>4460</v>
       </c>
-      <c r="P82" s="61">
-        <f t="shared" si="2"/>
+      <c r="P82" s="60">
+        <f t="shared" si="4"/>
         <v>4615</v>
       </c>
-      <c r="Q82" s="61">
-        <f t="shared" si="2"/>
+      <c r="Q82" s="60">
+        <f t="shared" si="4"/>
         <v>5425</v>
       </c>
     </row>
     <row r="83" spans="3:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C83" s="53"/>
-      <c r="D83" s="54"/>
-      <c r="E83" s="55"/>
-      <c r="F83" s="62"/>
-      <c r="G83" s="62"/>
-      <c r="H83" s="62"/>
-      <c r="I83" s="62"/>
-      <c r="J83" s="62"/>
-      <c r="K83" s="62"/>
-      <c r="L83" s="62"/>
-      <c r="M83" s="62"/>
-      <c r="N83" s="62"/>
-      <c r="O83" s="62"/>
-      <c r="P83" s="62"/>
-      <c r="Q83" s="62"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="52"/>
+      <c r="E83" s="53"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
+      <c r="H83" s="61"/>
+      <c r="I83" s="61"/>
+      <c r="J83" s="61"/>
+      <c r="K83" s="61"/>
+      <c r="L83" s="61"/>
+      <c r="M83" s="61"/>
+      <c r="N83" s="61"/>
+      <c r="O83" s="61"/>
+      <c r="P83" s="61"/>
+      <c r="Q83" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="252">
@@ -8780,7 +8852,7 @@
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C25" s="58"/>
+      <c r="C25" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>